<commit_message>
Testing and reporting issues
</commit_message>
<xml_diff>
--- a/employee-details.xlsx
+++ b/employee-details.xlsx
@@ -5,23 +5,37 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://merrakyindia-my.sharepoint.com/personal/bhagavan_prasad_merraky_com/Documents/docs/auto-reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dump\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_A6A1A54802DED85D54397E2594FF74CADCC441C1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{783E60AB-B937-493E-B560-621126362A0A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9BBC5C-AAF4-44F4-B821-A84FA78B023F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="02-stories" sheetId="2" r:id="rId1"/>
     <sheet name="01-epics" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'02-stories'!$A$1:$N$23</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="86">
   <si>
     <t>#</t>
   </si>
@@ -29,111 +43,24 @@
     <t>PCS-28018</t>
   </si>
   <si>
-    <t>PCS-2122</t>
-  </si>
-  <si>
-    <t>PCS-27974</t>
-  </si>
-  <si>
-    <t>QA: Testing the throughput with standard/less packet sizes/varied user load in ESP mode</t>
-  </si>
-  <si>
     <t>balachandras</t>
   </si>
   <si>
-    <t>PCS-27972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QA:SM HW : ESP Max Users/Tunnel Setup count </t>
-  </si>
-  <si>
-    <t>PCS-27539</t>
-  </si>
-  <si>
-    <t>Planning to validate RAID and LVM testing</t>
-  </si>
-  <si>
-    <t>PCS-25735</t>
-  </si>
-  <si>
-    <t>QA: Testing the HW-RAID controller functionality</t>
-  </si>
-  <si>
     <t>PCS-28042</t>
   </si>
   <si>
-    <t>PCS-28004</t>
-  </si>
-  <si>
-    <t>SM HW - ISA8000F Platform Testing, Code Review</t>
-  </si>
-  <si>
     <t>balajit</t>
   </si>
   <si>
-    <t>PCS-28003</t>
-  </si>
-  <si>
-    <t>SM HW - ISA8000F Platform addition - License and UI Changes</t>
-  </si>
-  <si>
-    <t>PCS-28002</t>
-  </si>
-  <si>
-    <t>SM HW - ISA8000F Platform addition - Platform changes</t>
-  </si>
-  <si>
     <t>PCS-28017</t>
   </si>
   <si>
-    <t>PCS-27971</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SM-HW : ISA8000 - Make Coreboot/init changes as platform specific  </t>
-  </si>
-  <si>
     <t>kalaimani.k</t>
   </si>
   <si>
-    <t>PCS-27007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SM-HW: ISA8000 Upgrade and Rollover Confirmation with LVM </t>
-  </si>
-  <si>
-    <t>PCS-27969</t>
-  </si>
-  <si>
-    <t>LVM: Support and bug fixes</t>
-  </si>
-  <si>
-    <t>PCS-27566</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QA: SMHW: Tunnel setup rate test for 25k Users on SSL mode </t>
-  </si>
-  <si>
     <t>karthikr</t>
   </si>
   <si>
-    <t>PCS-27538</t>
-  </si>
-  <si>
-    <t>QA: SM HW : Perform throughput tests with IMIX traffic(SSL)</t>
-  </si>
-  <si>
-    <t>PCS-27978</t>
-  </si>
-  <si>
-    <t>QA: SM HW : SSL Max Throughput (25k Users/Tunnels, 1350 bytes)</t>
-  </si>
-  <si>
-    <t>PCS-27975</t>
-  </si>
-  <si>
-    <t>QA: Build image from Build plan</t>
-  </si>
-  <si>
     <t>Issue key</t>
   </si>
   <si>
@@ -152,9 +79,6 @@
     <t>Custom field (Story Points)</t>
   </si>
   <si>
-    <t>teste</t>
-  </si>
-  <si>
     <t>Original Estimate</t>
   </si>
   <si>
@@ -179,9 +103,6 @@
     <t>May21-Performance</t>
   </si>
   <si>
-    <t>PCS-2112</t>
-  </si>
-  <si>
     <t>May21-ISA8000x-Support</t>
   </si>
   <si>
@@ -222,6 +143,156 @@
   </si>
   <si>
     <t>May21-Baseline</t>
+  </si>
+  <si>
+    <t>PCS-28233</t>
+  </si>
+  <si>
+    <t>ssubramanian</t>
+  </si>
+  <si>
+    <t>PCS-28264</t>
+  </si>
+  <si>
+    <t>PCS-28333</t>
+  </si>
+  <si>
+    <t>PCS-27371</t>
+  </si>
+  <si>
+    <t>PCS-27022</t>
+  </si>
+  <si>
+    <t>rajeshg</t>
+  </si>
+  <si>
+    <t>PCS-28232</t>
+  </si>
+  <si>
+    <t>PCS-28332</t>
+  </si>
+  <si>
+    <t>PCS-28312</t>
+  </si>
+  <si>
+    <t>praveens</t>
+  </si>
+  <si>
+    <t>PCS-28318</t>
+  </si>
+  <si>
+    <t>PCS-28319</t>
+  </si>
+  <si>
+    <t>PCS-28441</t>
+  </si>
+  <si>
+    <t>PCS-28313</t>
+  </si>
+  <si>
+    <t>PCS-28315</t>
+  </si>
+  <si>
+    <t>PCS-26807</t>
+  </si>
+  <si>
+    <t>PCS-28334</t>
+  </si>
+  <si>
+    <t>PCS-28663</t>
+  </si>
+  <si>
+    <t>PCS-28355</t>
+  </si>
+  <si>
+    <t>PCS-28357</t>
+  </si>
+  <si>
+    <t>PCS-28390</t>
+  </si>
+  <si>
+    <t>PCS-28314</t>
+  </si>
+  <si>
+    <t>PCS-28316</t>
+  </si>
+  <si>
+    <t>PCS-28438</t>
+  </si>
+  <si>
+    <t>PCS-2124</t>
+  </si>
+  <si>
+    <t>[ISA8K]: System is allowing more than permitted Licenses</t>
+  </si>
+  <si>
+    <t>[ISA8K-F]:Able to establish 25K Tunnels without licenses</t>
+  </si>
+  <si>
+    <t>ISA8K Platform porting document-part1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM HW: Licensing Dev Information Documentation </t>
+  </si>
+  <si>
+    <t>SuperDoctor: Confirm SuperDoctor diagnostic tool with SM-HW port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ISA8K]: HW status &amp; other information missing from Admin UI </t>
+  </si>
+  <si>
+    <t>PCS-2126</t>
+  </si>
+  <si>
+    <t>SM-HW: Pixe Packaging - Testing on HW</t>
+  </si>
+  <si>
+    <t>QA-ISA8K-Perf Baseline: Max Users/Tunnel Setup count(ESP)</t>
+  </si>
+  <si>
+    <t>QA-ISA8K-Perf Baseline: Tunnel setup rate tests(ESP)</t>
+  </si>
+  <si>
+    <t>QA-ISA8K-Perf Baseline: Baseline the Max Throughput(ESP)</t>
+  </si>
+  <si>
+    <t>[SM-HW]: Investigate the issue where admin UI is not accessible on HW 38</t>
+  </si>
+  <si>
+    <t>QA-ISA8K-Perf Baseline: Max Users/Tunnel Setup count(SSL)</t>
+  </si>
+  <si>
+    <t>QA-ISA8K-Perf Baseline: Baseline the Max Throughput(SSL)</t>
+  </si>
+  <si>
+    <t>PCS-2114</t>
+  </si>
+  <si>
+    <t>SMHW: Checking BIOS configuration</t>
+  </si>
+  <si>
+    <t>ISA8K Platform porting document (Driver related)</t>
+  </si>
+  <si>
+    <t>SM-HW: Analysis and Explore the Secure Boot option on SM HW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM-HW: ISA8000 License parameters information collection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM HW: CPU Affinity Usage Checking during traffic </t>
+  </si>
+  <si>
+    <t>SM-HW: ISA8000 License checking support</t>
+  </si>
+  <si>
+    <t>QA-ISA8K-Perf Baseline: Tunnel setup rate tests(SSL)</t>
+  </si>
+  <si>
+    <t>QA-ISA8K-Perf Baseline: Throughput-Standard/less packet sizes/varied user load(SSL)</t>
+  </si>
+  <si>
+    <t>[SM HW]: Flashing serial number to BIOS</t>
   </si>
 </sst>
 </file>
@@ -540,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,79 +625,81 @@
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="81.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="81.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C2">
-        <v>594882</v>
+        <v>596065</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>57600</v>
       </c>
       <c r="I2">
         <v>57600</v>
@@ -634,499 +707,830 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>57600</v>
-      </c>
-      <c r="L2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C3">
-        <v>594870</v>
+        <v>596185</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
+      <c r="H3">
+        <v>57600</v>
+      </c>
       <c r="I3">
         <v>57600</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>57600</v>
-      </c>
-      <c r="L3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C4">
-        <v>593251</v>
+        <v>596498</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>86400</v>
       </c>
       <c r="I4">
-        <v>57600</v>
+        <v>86400</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4">
-        <v>57600</v>
-      </c>
-      <c r="L4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C5">
-        <v>583642</v>
+        <v>592012</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
+      <c r="H5">
+        <v>57600</v>
+      </c>
       <c r="I5">
         <v>57600</v>
       </c>
       <c r="J5">
-        <v>43200</v>
-      </c>
-      <c r="K5">
-        <v>57600</v>
-      </c>
-      <c r="L5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C6">
-        <v>594947</v>
+        <v>590514</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>86400</v>
       </c>
       <c r="I6">
-        <v>57600</v>
-      </c>
-      <c r="K6">
-        <v>57600</v>
+        <v>64800</v>
+      </c>
+      <c r="J6">
+        <v>21600</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
       </c>
       <c r="L6" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="M6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C7">
-        <v>594946</v>
+        <v>596064</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="G7">
         <v>4</v>
       </c>
+      <c r="H7">
+        <v>57600</v>
+      </c>
       <c r="I7">
-        <v>57600</v>
-      </c>
-      <c r="K7">
-        <v>57600</v>
-      </c>
-      <c r="L7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>115200</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C8">
-        <v>594945</v>
+        <v>596496</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="G8">
         <v>6</v>
       </c>
+      <c r="H8">
+        <v>86400</v>
+      </c>
       <c r="I8">
-        <v>86400</v>
+        <v>10800</v>
       </c>
       <c r="J8">
-        <v>82800</v>
-      </c>
-      <c r="K8">
-        <v>3600</v>
+        <v>75600</v>
+      </c>
+      <c r="K8" t="s">
+        <v>61</v>
       </c>
       <c r="L8" t="s">
-        <v>2</v>
-      </c>
-      <c r="O8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="N8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C9">
-        <v>594869</v>
+        <v>596429</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="G9">
         <v>4</v>
       </c>
+      <c r="H9">
+        <v>57600</v>
+      </c>
       <c r="I9">
-        <v>57600</v>
+        <v>115200</v>
       </c>
       <c r="J9">
-        <v>57600</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>2</v>
-      </c>
-      <c r="O9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C10">
-        <v>590473</v>
+        <v>596435</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="G10">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>57600</v>
       </c>
       <c r="I10">
-        <v>115200</v>
+        <v>57600</v>
       </c>
       <c r="J10">
-        <v>28800</v>
-      </c>
-      <c r="K10">
-        <v>86400</v>
-      </c>
-      <c r="L10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M10" t="s">
-        <v>56</v>
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
       </c>
       <c r="N10" t="s">
-        <v>2</v>
-      </c>
-      <c r="O10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C11">
-        <v>594853</v>
+        <v>596436</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>86400</v>
       </c>
       <c r="I11">
-        <v>57600</v>
-      </c>
-      <c r="K11">
-        <v>57600</v>
-      </c>
-      <c r="L11" t="s">
-        <v>2</v>
-      </c>
-      <c r="O11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>86400</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C12">
-        <v>593427</v>
+        <v>596948</v>
       </c>
       <c r="D12" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>28800</v>
       </c>
       <c r="I12">
-        <v>28800</v>
-      </c>
-      <c r="K12">
-        <v>28800</v>
-      </c>
-      <c r="L12" t="s">
-        <v>2</v>
-      </c>
-      <c r="O12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>50400</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C13">
-        <v>593250</v>
+        <v>596430</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G13">
         <v>4</v>
       </c>
+      <c r="H13">
+        <v>7200</v>
+      </c>
       <c r="I13">
-        <v>57600</v>
-      </c>
-      <c r="K13">
-        <v>57600</v>
-      </c>
-      <c r="L13" t="s">
-        <v>2</v>
-      </c>
-      <c r="O13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>115200</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C14">
-        <v>594893</v>
+        <v>596432</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>86400</v>
       </c>
       <c r="I14">
-        <v>57600</v>
-      </c>
-      <c r="K14">
-        <v>57600</v>
+        <v>28800</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>61</v>
       </c>
       <c r="L14" t="s">
-        <v>2</v>
-      </c>
-      <c r="O14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="N14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C15">
-        <v>594885</v>
+        <v>589433</v>
       </c>
       <c r="D15" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>115200</v>
       </c>
       <c r="I15">
         <v>28800</v>
       </c>
       <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16">
+        <v>596499</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>86400</v>
+      </c>
+      <c r="I16">
+        <v>172800</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17">
+        <v>597761</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>1200</v>
+      </c>
+      <c r="I17">
+        <v>57600</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18">
+        <v>596647</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>86400</v>
+      </c>
+      <c r="I18">
+        <v>104400</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19">
+        <v>596652</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>86400</v>
+      </c>
+      <c r="I19">
+        <v>57600</v>
+      </c>
+      <c r="J19">
+        <v>28800</v>
+      </c>
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20">
+        <v>596746</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>57600</v>
+      </c>
+      <c r="I20">
+        <v>57600</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21">
+        <v>596431</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>86400</v>
+      </c>
+      <c r="I21">
+        <v>57600</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L21" t="s">
+        <v>68</v>
+      </c>
+      <c r="N21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22">
+        <v>596433</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>8</v>
+      </c>
+      <c r="H22">
         <v>14400</v>
       </c>
-      <c r="K15">
-        <v>14400</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="I22">
+        <v>144000</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>61</v>
+      </c>
+      <c r="L22" t="s">
+        <v>68</v>
+      </c>
+      <c r="N22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23">
+        <v>596940</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
         <v>2</v>
       </c>
-      <c r="O15" t="s">
-        <v>36</v>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>28800</v>
+      </c>
+      <c r="I23">
+        <v>57600</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1138,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,22 +1559,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1181,7 +1585,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1">
         <v>44336</v>
@@ -1201,10 +1605,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1">
         <v>44336</v>
@@ -1224,10 +1628,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1">
         <v>44336</v>
@@ -1247,10 +1651,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1">
         <v>44336</v>
@@ -1270,10 +1674,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1">
         <v>44336</v>
@@ -1293,10 +1697,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1">
         <v>44320</v>
@@ -1307,7 +1711,9 @@
       <c r="F7" s="1">
         <v>44320</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>44364</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
defined seperate function for formulae and gave formulae to every cell in sheet
</commit_message>
<xml_diff>
--- a/employee-details.xlsx
+++ b/employee-details.xlsx
@@ -640,11 +640,13 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L3" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>0</v>
+      <c r="L3" s="1">
+        <f>K3/3600</f>
+        <v/>
+      </c>
+      <c r="M3" s="1">
+        <f>J3-L3</f>
+        <v/>
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
@@ -657,7 +659,7 @@
         </is>
       </c>
       <c r="P3" s="1">
-        <f>L3/J3*100</f>
+        <f>J3/L3%</f>
         <v/>
       </c>
       <c r="Q3" s="1" t="inlineStr">
@@ -725,11 +727,12 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L4" s="1" t="n">
-        <v>16</v>
+      <c r="L4" s="1">
+        <f>K4/3600</f>
+        <v/>
       </c>
       <c r="M4" s="1">
-        <f>J3-L3</f>
+        <f>J4-L4</f>
         <v/>
       </c>
       <c r="N4" s="1" t="inlineStr">
@@ -742,10 +745,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P4" s="1" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="P4" s="1">
+        <f>J4/L4%</f>
+        <v/>
       </c>
       <c r="Q4" s="1" t="inlineStr">
         <is>
@@ -812,11 +814,13 @@
           <t>86400</t>
         </is>
       </c>
-      <c r="L5" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="M5" s="1" t="n">
-        <v>0</v>
+      <c r="L5" s="1">
+        <f>K5/3600</f>
+        <v/>
+      </c>
+      <c r="M5" s="1">
+        <f>J5-L5</f>
+        <v/>
       </c>
       <c r="N5" s="1" t="inlineStr">
         <is>
@@ -828,10 +832,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P5" s="1" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="P5" s="1">
+        <f>J5/L5%</f>
+        <v/>
       </c>
       <c r="Q5" s="1" t="inlineStr">
         <is>
@@ -898,11 +901,13 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L6" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>0</v>
+      <c r="L6" s="1">
+        <f>K6/3600</f>
+        <v/>
+      </c>
+      <c r="M6" s="1">
+        <f>J6-L6</f>
+        <v/>
       </c>
       <c r="N6" s="1" t="inlineStr">
         <is>
@@ -914,10 +919,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P6" s="1" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="P6" s="1">
+        <f>J6/L6%</f>
+        <v/>
       </c>
       <c r="Q6" s="1" t="inlineStr">
         <is>
@@ -984,11 +988,13 @@
           <t>64800</t>
         </is>
       </c>
-      <c r="L7" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="M7" s="1" t="n">
-        <v>6</v>
+      <c r="L7" s="1">
+        <f>K7/3600</f>
+        <v/>
+      </c>
+      <c r="M7" s="1">
+        <f>J7-L7</f>
+        <v/>
       </c>
       <c r="N7" s="1" t="inlineStr">
         <is>
@@ -1000,10 +1006,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P7" s="1" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
+      <c r="P7" s="1">
+        <f>J7/L7%</f>
+        <v/>
       </c>
       <c r="Q7" s="1" t="inlineStr">
         <is>
@@ -1070,11 +1075,13 @@
           <t>115200</t>
         </is>
       </c>
-      <c r="L8" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <v>-16</v>
+      <c r="L8" s="1">
+        <f>K8/3600</f>
+        <v/>
+      </c>
+      <c r="M8" s="1">
+        <f>J8-L8</f>
+        <v/>
       </c>
       <c r="N8" s="1" t="inlineStr">
         <is>
@@ -1086,10 +1093,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P8" s="1" t="inlineStr">
-        <is>
-          <t>200%</t>
-        </is>
+      <c r="P8" s="1">
+        <f>J8/L8%</f>
+        <v/>
       </c>
       <c r="Q8" s="1" t="inlineStr">
         <is>
@@ -1156,11 +1162,13 @@
           <t>10800</t>
         </is>
       </c>
-      <c r="L9" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M9" s="1" t="n">
-        <v>21</v>
+      <c r="L9" s="1">
+        <f>K9/3600</f>
+        <v/>
+      </c>
+      <c r="M9" s="1">
+        <f>J9-L9</f>
+        <v/>
       </c>
       <c r="N9" s="1" t="inlineStr">
         <is>
@@ -1172,10 +1180,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P9" s="1" t="inlineStr">
-        <is>
-          <t>12%</t>
-        </is>
+      <c r="P9" s="1">
+        <f>J9/L9%</f>
+        <v/>
       </c>
       <c r="Q9" s="1" t="inlineStr">
         <is>
@@ -1242,11 +1249,13 @@
           <t>115200</t>
         </is>
       </c>
-      <c r="L10" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="M10" s="1" t="n">
-        <v>-16</v>
+      <c r="L10" s="1">
+        <f>K10/3600</f>
+        <v/>
+      </c>
+      <c r="M10" s="1">
+        <f>J10-L10</f>
+        <v/>
       </c>
       <c r="N10" s="1" t="inlineStr">
         <is>
@@ -1258,10 +1267,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P10" s="1" t="inlineStr">
-        <is>
-          <t>200%</t>
-        </is>
+      <c r="P10" s="1">
+        <f>J10/L10%</f>
+        <v/>
       </c>
       <c r="Q10" s="1" t="inlineStr">
         <is>
@@ -1328,11 +1336,13 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L11" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="M11" s="1" t="n">
-        <v>0</v>
+      <c r="L11" s="1">
+        <f>K11/3600</f>
+        <v/>
+      </c>
+      <c r="M11" s="1">
+        <f>J11-L11</f>
+        <v/>
       </c>
       <c r="N11" s="1" t="inlineStr">
         <is>
@@ -1344,10 +1354,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P11" s="1" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="P11" s="1">
+        <f>J11/L11%</f>
+        <v/>
       </c>
       <c r="Q11" s="1" t="inlineStr">
         <is>
@@ -1414,11 +1423,13 @@
           <t>86400</t>
         </is>
       </c>
-      <c r="L12" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="M12" s="1" t="n">
-        <v>0</v>
+      <c r="L12" s="1">
+        <f>K12/3600</f>
+        <v/>
+      </c>
+      <c r="M12" s="1">
+        <f>J12-L12</f>
+        <v/>
       </c>
       <c r="N12" s="1" t="inlineStr">
         <is>
@@ -1430,10 +1441,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P12" s="1" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="P12" s="1">
+        <f>J12/L12%</f>
+        <v/>
       </c>
       <c r="Q12" s="1" t="inlineStr">
         <is>
@@ -1500,11 +1510,13 @@
           <t>50400</t>
         </is>
       </c>
-      <c r="L13" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>-6</v>
+      <c r="L13" s="1">
+        <f>K13/3600</f>
+        <v/>
+      </c>
+      <c r="M13" s="1">
+        <f>J13-L13</f>
+        <v/>
       </c>
       <c r="N13" s="1" t="inlineStr">
         <is>
@@ -1516,10 +1528,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P13" s="1" t="inlineStr">
-        <is>
-          <t>175%</t>
-        </is>
+      <c r="P13" s="1">
+        <f>J13/L13%</f>
+        <v/>
       </c>
       <c r="Q13" s="1" t="inlineStr">
         <is>
@@ -1586,11 +1597,13 @@
           <t>115200</t>
         </is>
       </c>
-      <c r="L14" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="M14" s="1" t="n">
-        <v>-30</v>
+      <c r="L14" s="1">
+        <f>K14/3600</f>
+        <v/>
+      </c>
+      <c r="M14" s="1">
+        <f>J14-L14</f>
+        <v/>
       </c>
       <c r="N14" s="1" t="inlineStr">
         <is>
@@ -1602,10 +1615,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P14" s="1" t="inlineStr">
-        <is>
-          <t>1600%</t>
-        </is>
+      <c r="P14" s="1">
+        <f>J14/L14%</f>
+        <v/>
       </c>
       <c r="Q14" s="1" t="inlineStr">
         <is>
@@ -1672,11 +1684,13 @@
           <t>28800</t>
         </is>
       </c>
-      <c r="L15" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="M15" s="1" t="n">
-        <v>16</v>
+      <c r="L15" s="1">
+        <f>K15/3600</f>
+        <v/>
+      </c>
+      <c r="M15" s="1">
+        <f>J15-L15</f>
+        <v/>
       </c>
       <c r="N15" s="1" t="inlineStr">
         <is>
@@ -1688,10 +1702,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P15" s="1" t="inlineStr">
-        <is>
-          <t>33%</t>
-        </is>
+      <c r="P15" s="1">
+        <f>J15/L15%</f>
+        <v/>
       </c>
       <c r="Q15" s="1" t="inlineStr">
         <is>
@@ -1758,11 +1771,13 @@
           <t>28800</t>
         </is>
       </c>
-      <c r="L16" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="M16" s="1" t="n">
-        <v>24</v>
+      <c r="L16" s="1">
+        <f>K16/3600</f>
+        <v/>
+      </c>
+      <c r="M16" s="1">
+        <f>J16-L16</f>
+        <v/>
       </c>
       <c r="N16" s="1" t="inlineStr">
         <is>
@@ -1774,10 +1789,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P16" s="1" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="P16" s="1">
+        <f>J16/L16%</f>
+        <v/>
       </c>
       <c r="Q16" s="1" t="inlineStr">
         <is>
@@ -1844,11 +1858,13 @@
           <t>172800</t>
         </is>
       </c>
-      <c r="L17" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="M17" s="1" t="n">
-        <v>-24</v>
+      <c r="L17" s="1">
+        <f>K17/3600</f>
+        <v/>
+      </c>
+      <c r="M17" s="1">
+        <f>J17-L17</f>
+        <v/>
       </c>
       <c r="N17" s="1" t="inlineStr">
         <is>
@@ -1860,10 +1876,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P17" s="1" t="inlineStr">
-        <is>
-          <t>200%</t>
-        </is>
+      <c r="P17" s="1">
+        <f>J17/L17%</f>
+        <v/>
       </c>
       <c r="Q17" s="1" t="inlineStr">
         <is>
@@ -1930,11 +1945,13 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="M18" s="1" t="n">
-        <v>-15.66666666666667</v>
+      <c r="L18" s="1">
+        <f>K18/3600</f>
+        <v/>
+      </c>
+      <c r="M18" s="1">
+        <f>J18-L18</f>
+        <v/>
       </c>
       <c r="N18" s="1" t="inlineStr">
         <is>
@@ -1946,10 +1963,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P18" s="1" t="inlineStr">
-        <is>
-          <t>4800%</t>
-        </is>
+      <c r="P18" s="1">
+        <f>J18/L18%</f>
+        <v/>
       </c>
       <c r="Q18" s="1" t="inlineStr">
         <is>
@@ -2016,11 +2032,13 @@
           <t>104400</t>
         </is>
       </c>
-      <c r="L19" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="M19" s="1" t="n">
-        <v>-5</v>
+      <c r="L19" s="1">
+        <f>K19/3600</f>
+        <v/>
+      </c>
+      <c r="M19" s="1">
+        <f>J19-L19</f>
+        <v/>
       </c>
       <c r="N19" s="1" t="inlineStr">
         <is>
@@ -2032,10 +2050,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P19" s="1" t="inlineStr">
-        <is>
-          <t>121%</t>
-        </is>
+      <c r="P19" s="1">
+        <f>J19/L19%</f>
+        <v/>
       </c>
       <c r="Q19" s="1" t="inlineStr">
         <is>
@@ -2102,11 +2119,13 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L20" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="M20" s="1" t="n">
-        <v>8</v>
+      <c r="L20" s="1">
+        <f>K20/3600</f>
+        <v/>
+      </c>
+      <c r="M20" s="1">
+        <f>J20-L20</f>
+        <v/>
       </c>
       <c r="N20" s="1" t="inlineStr">
         <is>
@@ -2118,10 +2137,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P20" s="1" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
+      <c r="P20" s="1">
+        <f>J20/L20%</f>
+        <v/>
       </c>
       <c r="Q20" s="1" t="inlineStr">
         <is>
@@ -2188,11 +2206,13 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L21" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="M21" s="1" t="n">
-        <v>0</v>
+      <c r="L21" s="1">
+        <f>K21/3600</f>
+        <v/>
+      </c>
+      <c r="M21" s="1">
+        <f>J21-L21</f>
+        <v/>
       </c>
       <c r="N21" s="1" t="inlineStr">
         <is>
@@ -2204,10 +2224,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P21" s="1" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="P21" s="1">
+        <f>J21/L21%</f>
+        <v/>
       </c>
       <c r="Q21" s="1" t="inlineStr">
         <is>
@@ -2274,11 +2293,13 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L22" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="M22" s="1" t="n">
-        <v>8</v>
+      <c r="L22" s="1">
+        <f>K22/3600</f>
+        <v/>
+      </c>
+      <c r="M22" s="1">
+        <f>J22-L22</f>
+        <v/>
       </c>
       <c r="N22" s="1" t="inlineStr">
         <is>
@@ -2290,10 +2311,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P22" s="1" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
+      <c r="P22" s="1">
+        <f>J22/L22%</f>
+        <v/>
       </c>
       <c r="Q22" s="1" t="inlineStr">
         <is>
@@ -2360,11 +2380,13 @@
           <t>144000</t>
         </is>
       </c>
-      <c r="L23" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="M23" s="1" t="n">
-        <v>-36</v>
+      <c r="L23" s="1">
+        <f>K23/3600</f>
+        <v/>
+      </c>
+      <c r="M23" s="1">
+        <f>J23-L23</f>
+        <v/>
       </c>
       <c r="N23" s="1" t="inlineStr">
         <is>
@@ -2376,10 +2398,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P23" s="1" t="inlineStr">
-        <is>
-          <t>1000%</t>
-        </is>
+      <c r="P23" s="1">
+        <f>J23/L23%</f>
+        <v/>
       </c>
       <c r="Q23" s="1" t="inlineStr">
         <is>
@@ -2446,11 +2467,13 @@
           <t>57600</t>
         </is>
       </c>
-      <c r="L24" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="M24" s="1" t="n">
-        <v>-8</v>
+      <c r="L24" s="1">
+        <f>K24/3600</f>
+        <v/>
+      </c>
+      <c r="M24" s="1">
+        <f>J24-L24</f>
+        <v/>
       </c>
       <c r="N24" s="1" t="inlineStr">
         <is>
@@ -2462,10 +2485,9 @@
           <t>5/20/2021</t>
         </is>
       </c>
-      <c r="P24" s="1" t="inlineStr">
-        <is>
-          <t>200%</t>
-        </is>
+      <c r="P24" s="1">
+        <f>J24/L24%</f>
+        <v/>
       </c>
       <c r="Q24" s="1" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
text-alignment function is added to the project
</commit_message>
<xml_diff>
--- a/employee-details.xlsx
+++ b/employee-details.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7365" windowWidth="19815" xWindow="390" yWindow="555"/>
   </bookViews>
   <sheets>
     <sheet name="generated" sheetId="1" state="visible" r:id="rId1"/>
@@ -64,36 +64,36 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -470,7 +470,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="n"/>
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>S.No</t>
+        </is>
+      </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
           <t>EPIC ID</t>
@@ -597,7 +601,7 @@
           <t>PCS-28016</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -672,6 +676,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -684,7 +689,7 @@
           <t>PCS-28016</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -759,6 +764,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -771,7 +777,7 @@
           <t>PCS-28322</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -846,6 +852,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -858,7 +865,7 @@
           <t>PCS-28322</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -933,6 +940,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S6" s="1" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -945,7 +953,7 @@
           <t>PCS-28017</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1020,6 +1028,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1032,7 +1041,7 @@
           <t>PCS-28017</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1107,6 +1116,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1119,7 +1129,7 @@
           <t>PCS-28017</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="1" t="inlineStr">
         <is>
           <t>PCS-2126</t>
         </is>
@@ -1194,6 +1204,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1206,7 +1217,7 @@
           <t>PCS-28311</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1281,6 +1292,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1293,7 +1305,7 @@
           <t>PCS-28311</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1368,6 +1380,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1380,7 +1393,7 @@
           <t>PCS-28311</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1455,6 +1468,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S12" s="1" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1467,7 +1481,7 @@
           <t>PCS-28322</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1542,6 +1556,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S13" s="1" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1554,7 +1569,7 @@
           <t>PCS-28311</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1629,6 +1644,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1641,7 +1657,7 @@
           <t>PCS-28311</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="1" t="inlineStr">
         <is>
           <t>PCS-2126</t>
         </is>
@@ -1716,6 +1732,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S15" s="1" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1728,7 +1745,7 @@
           <t>PCS-28017</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1803,6 +1820,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S16" s="1" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1815,7 +1833,7 @@
           <t>PCS-28322</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1890,6 +1908,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1902,7 +1921,7 @@
           <t>PCS-28322</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -1977,6 +1996,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S18" s="1" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1989,7 +2009,7 @@
           <t>PCS-28016</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -2064,6 +2084,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S19" s="1" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -2076,7 +2097,7 @@
           <t>PCS-28016</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -2151,6 +2172,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -2163,7 +2185,7 @@
           <t>PCS-28016</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -2238,6 +2260,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S21" s="1" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -2250,7 +2273,7 @@
           <t>PCS-28311</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="1" t="inlineStr">
         <is>
           <t>PCS-2126</t>
         </is>
@@ -2325,6 +2348,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S22" s="1" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -2337,7 +2361,7 @@
           <t>PCS-28311</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="1" t="inlineStr">
         <is>
           <t>PCS-2126</t>
         </is>
@@ -2412,6 +2436,7 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -2424,7 +2449,7 @@
           <t>PCS-28322</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="1" t="inlineStr">
         <is>
           <t>PCS-2124</t>
         </is>
@@ -2499,12 +2524,13 @@
           <t>0%</t>
         </is>
       </c>
+      <c r="S24" s="1" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:S1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2522,6 +2548,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
definied code with functions
</commit_message>
<xml_diff>
--- a/employee-details.xlsx
+++ b/employee-details.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7365" windowWidth="19815" xWindow="390" yWindow="555"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="generated" sheetId="1" state="visible" r:id="rId1"/>
@@ -64,36 +64,36 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -470,11 +470,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="inlineStr">
-        <is>
-          <t>S.No</t>
-        </is>
-      </c>
+      <c r="A2" s="8" t="n"/>
       <c r="B2" s="8" t="inlineStr">
         <is>
           <t>EPIC ID</t>
@@ -654,12 +650,12 @@
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O3" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P3" s="1">
@@ -742,12 +738,12 @@
       </c>
       <c r="N4" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O4" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P4" s="1">
@@ -830,12 +826,12 @@
       </c>
       <c r="N5" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O5" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P5" s="1">
@@ -918,12 +914,12 @@
       </c>
       <c r="N6" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O6" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P6" s="1">
@@ -1006,12 +1002,12 @@
       </c>
       <c r="N7" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O7" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P7" s="1">
@@ -1094,12 +1090,12 @@
       </c>
       <c r="N8" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O8" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P8" s="1">
@@ -1182,12 +1178,12 @@
       </c>
       <c r="N9" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O9" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P9" s="1">
@@ -1270,12 +1266,12 @@
       </c>
       <c r="N10" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O10" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P10" s="1">
@@ -1358,12 +1354,12 @@
       </c>
       <c r="N11" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O11" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P11" s="1">
@@ -1446,12 +1442,12 @@
       </c>
       <c r="N12" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O12" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P12" s="1">
@@ -1534,12 +1530,12 @@
       </c>
       <c r="N13" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O13" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P13" s="1">
@@ -1622,12 +1618,12 @@
       </c>
       <c r="N14" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O14" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P14" s="1">
@@ -1710,12 +1706,12 @@
       </c>
       <c r="N15" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O15" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P15" s="1">
@@ -1798,12 +1794,12 @@
       </c>
       <c r="N16" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O16" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P16" s="1">
@@ -1886,12 +1882,12 @@
       </c>
       <c r="N17" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O17" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P17" s="1">
@@ -1974,12 +1970,12 @@
       </c>
       <c r="N18" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O18" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P18" s="1">
@@ -2062,12 +2058,12 @@
       </c>
       <c r="N19" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O19" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P19" s="1">
@@ -2150,12 +2146,12 @@
       </c>
       <c r="N20" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O20" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P20" s="1">
@@ -2238,12 +2234,12 @@
       </c>
       <c r="N21" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O21" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P21" s="1">
@@ -2326,12 +2322,12 @@
       </c>
       <c r="N22" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O22" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P22" s="1">
@@ -2414,12 +2410,12 @@
       </c>
       <c r="N23" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O23" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P23" s="1">
@@ -2502,12 +2498,12 @@
       </c>
       <c r="N24" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="O24" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="P24" s="1">
@@ -2530,7 +2526,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:S1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2548,6 +2544,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed text to numbers
</commit_message>
<xml_diff>
--- a/employee-details.xlsx
+++ b/employee-details.xlsx
@@ -470,7 +470,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="n"/>
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>S.No</t>
+        </is>
+      </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
           <t>EPIC ID</t>
@@ -587,10 +591,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
@@ -617,10 +619,8 @@
           <t>ssubramanian</t>
         </is>
       </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G3" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
@@ -635,10 +635,8 @@
       <c r="J3" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K3" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L3" s="1">
         <f>K3/3600</f>
@@ -675,10 +673,8 @@
       <c r="S3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
@@ -705,10 +701,8 @@
           <t>ssubramanian</t>
         </is>
       </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G4" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H4" s="1" t="inlineStr">
         <is>
@@ -723,10 +717,8 @@
       <c r="J4" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K4" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L4" s="1">
         <f>K4/3600</f>
@@ -763,10 +755,8 @@
       <c r="S4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
@@ -793,10 +783,8 @@
           <t>ssubramanian</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G5" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
@@ -811,10 +799,8 @@
       <c r="J5" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>86400</t>
-        </is>
+      <c r="K5" s="1" t="n">
+        <v>86400</v>
       </c>
       <c r="L5" s="1">
         <f>K5/3600</f>
@@ -851,10 +837,8 @@
       <c r="S5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
@@ -881,10 +865,8 @@
           <t>ssubramanian</t>
         </is>
       </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
@@ -899,10 +881,8 @@
       <c r="J6" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K6" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L6" s="1">
         <f>K6/3600</f>
@@ -939,10 +919,8 @@
       <c r="S6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
@@ -969,10 +947,8 @@
           <t>rajeshg</t>
         </is>
       </c>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
@@ -987,10 +963,8 @@
       <c r="J7" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>64800</t>
-        </is>
+      <c r="K7" s="1" t="n">
+        <v>64800</v>
       </c>
       <c r="L7" s="1">
         <f>K7/3600</f>
@@ -1027,10 +1001,8 @@
       <c r="S7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
@@ -1057,10 +1029,8 @@
           <t>rajeshg</t>
         </is>
       </c>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G8" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H8" s="1" t="inlineStr">
         <is>
@@ -1075,10 +1045,8 @@
       <c r="J8" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K8" s="1" t="inlineStr">
-        <is>
-          <t>115200</t>
-        </is>
+      <c r="K8" s="1" t="n">
+        <v>115200</v>
       </c>
       <c r="L8" s="1">
         <f>K8/3600</f>
@@ -1115,10 +1083,8 @@
       <c r="S8" s="1" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
@@ -1145,10 +1111,8 @@
           <t>rajeshg</t>
         </is>
       </c>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G9" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H9" s="1" t="inlineStr">
         <is>
@@ -1163,10 +1127,8 @@
       <c r="J9" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K9" s="1" t="inlineStr">
-        <is>
-          <t>10800</t>
-        </is>
+      <c r="K9" s="1" t="n">
+        <v>10800</v>
       </c>
       <c r="L9" s="1">
         <f>K9/3600</f>
@@ -1203,10 +1165,8 @@
       <c r="S9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
@@ -1233,10 +1193,8 @@
           <t>praveens</t>
         </is>
       </c>
-      <c r="G10" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G10" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
@@ -1251,10 +1209,8 @@
       <c r="J10" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K10" s="1" t="inlineStr">
-        <is>
-          <t>115200</t>
-        </is>
+      <c r="K10" s="1" t="n">
+        <v>115200</v>
       </c>
       <c r="L10" s="1">
         <f>K10/3600</f>
@@ -1291,10 +1247,8 @@
       <c r="S10" s="1" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
@@ -1321,10 +1275,8 @@
           <t>praveens</t>
         </is>
       </c>
-      <c r="G11" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G11" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H11" s="1" t="inlineStr">
         <is>
@@ -1339,10 +1291,8 @@
       <c r="J11" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K11" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K11" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L11" s="1">
         <f>K11/3600</f>
@@ -1379,10 +1329,8 @@
       <c r="S11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
@@ -1409,10 +1357,8 @@
           <t>praveens</t>
         </is>
       </c>
-      <c r="G12" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G12" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H12" s="1" t="inlineStr">
         <is>
@@ -1427,10 +1373,8 @@
       <c r="J12" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K12" s="1" t="inlineStr">
-        <is>
-          <t>86400</t>
-        </is>
+      <c r="K12" s="1" t="n">
+        <v>86400</v>
       </c>
       <c r="L12" s="1">
         <f>K12/3600</f>
@@ -1467,10 +1411,8 @@
       <c r="S12" s="1" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
@@ -1497,10 +1439,8 @@
           <t>praveens</t>
         </is>
       </c>
-      <c r="G13" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="G13" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
@@ -1515,10 +1455,8 @@
       <c r="J13" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K13" s="1" t="inlineStr">
-        <is>
-          <t>50400</t>
-        </is>
+      <c r="K13" s="1" t="n">
+        <v>50400</v>
       </c>
       <c r="L13" s="1">
         <f>K13/3600</f>
@@ -1555,10 +1493,8 @@
       <c r="S13" s="1" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A14" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
@@ -1585,10 +1521,8 @@
           <t>karthikr</t>
         </is>
       </c>
-      <c r="G14" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G14" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H14" s="1" t="inlineStr">
         <is>
@@ -1603,10 +1537,8 @@
       <c r="J14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K14" s="1" t="inlineStr">
-        <is>
-          <t>115200</t>
-        </is>
+      <c r="K14" s="1" t="n">
+        <v>115200</v>
       </c>
       <c r="L14" s="1">
         <f>K14/3600</f>
@@ -1643,10 +1575,8 @@
       <c r="S14" s="1" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="A15" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
@@ -1673,10 +1603,8 @@
           <t>karthikr</t>
         </is>
       </c>
-      <c r="G15" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G15" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H15" s="1" t="inlineStr">
         <is>
@@ -1691,10 +1619,8 @@
       <c r="J15" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K15" s="1" t="inlineStr">
-        <is>
-          <t>28800</t>
-        </is>
+      <c r="K15" s="1" t="n">
+        <v>28800</v>
       </c>
       <c r="L15" s="1">
         <f>K15/3600</f>
@@ -1731,10 +1657,8 @@
       <c r="S15" s="1" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="A16" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
@@ -1761,10 +1685,8 @@
           <t>kalaimani.k</t>
         </is>
       </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="G16" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="H16" s="1" t="inlineStr">
         <is>
@@ -1779,10 +1701,8 @@
       <c r="J16" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="K16" s="1" t="inlineStr">
-        <is>
-          <t>28800</t>
-        </is>
+      <c r="K16" s="1" t="n">
+        <v>28800</v>
       </c>
       <c r="L16" s="1">
         <f>K16/3600</f>
@@ -1819,10 +1739,8 @@
       <c r="S16" s="1" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A17" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
@@ -1849,10 +1767,8 @@
           <t>kalaimani.k</t>
         </is>
       </c>
-      <c r="G17" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G17" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
@@ -1867,10 +1783,8 @@
       <c r="J17" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K17" s="1" t="inlineStr">
-        <is>
-          <t>172800</t>
-        </is>
+      <c r="K17" s="1" t="n">
+        <v>172800</v>
       </c>
       <c r="L17" s="1">
         <f>K17/3600</f>
@@ -1907,10 +1821,8 @@
       <c r="S17" s="1" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="A18" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
@@ -1937,10 +1849,8 @@
           <t>kalaimani.k</t>
         </is>
       </c>
-      <c r="G18" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G18" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H18" s="1" t="inlineStr">
         <is>
@@ -1955,10 +1865,8 @@
       <c r="J18" s="1" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="K18" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K18" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L18" s="1">
         <f>K18/3600</f>
@@ -1995,10 +1903,8 @@
       <c r="S18" s="1" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="A19" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
@@ -2025,10 +1931,8 @@
           <t>balajit</t>
         </is>
       </c>
-      <c r="G19" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G19" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H19" s="1" t="inlineStr">
         <is>
@@ -2043,10 +1947,8 @@
       <c r="J19" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K19" s="1" t="inlineStr">
-        <is>
-          <t>104400</t>
-        </is>
+      <c r="K19" s="1" t="n">
+        <v>104400</v>
       </c>
       <c r="L19" s="1">
         <f>K19/3600</f>
@@ -2083,10 +1985,8 @@
       <c r="S19" s="1" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="A20" s="1" t="n">
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
@@ -2113,10 +2013,8 @@
           <t>balajit</t>
         </is>
       </c>
-      <c r="G20" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G20" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H20" s="1" t="inlineStr">
         <is>
@@ -2131,10 +2029,8 @@
       <c r="J20" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K20" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K20" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L20" s="1">
         <f>K20/3600</f>
@@ -2171,10 +2067,8 @@
       <c r="S20" s="1" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="A21" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
@@ -2201,10 +2095,8 @@
           <t>balajit</t>
         </is>
       </c>
-      <c r="G21" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="G21" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="H21" s="1" t="inlineStr">
         <is>
@@ -2219,10 +2111,8 @@
       <c r="J21" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K21" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K21" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L21" s="1">
         <f>K21/3600</f>
@@ -2259,10 +2149,8 @@
       <c r="S21" s="1" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="A22" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
@@ -2289,10 +2177,8 @@
           <t>balachandras</t>
         </is>
       </c>
-      <c r="G22" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="G22" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="H22" s="1" t="inlineStr">
         <is>
@@ -2307,10 +2193,8 @@
       <c r="J22" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="K22" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K22" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L22" s="1">
         <f>K22/3600</f>
@@ -2347,10 +2231,8 @@
       <c r="S22" s="1" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="A23" s="1" t="n">
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
@@ -2377,10 +2259,8 @@
           <t>balachandras</t>
         </is>
       </c>
-      <c r="G23" s="1" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="G23" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="H23" s="1" t="inlineStr">
         <is>
@@ -2395,10 +2275,8 @@
       <c r="J23" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K23" s="1" t="inlineStr">
-        <is>
-          <t>144000</t>
-        </is>
+      <c r="K23" s="1" t="n">
+        <v>144000</v>
       </c>
       <c r="L23" s="1">
         <f>K23/3600</f>
@@ -2435,10 +2313,8 @@
       <c r="S23" s="1" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="A24" s="1" t="n">
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
@@ -2465,10 +2341,8 @@
           <t>balachandras</t>
         </is>
       </c>
-      <c r="G24" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="G24" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="H24" s="1" t="inlineStr">
         <is>
@@ -2483,10 +2357,8 @@
       <c r="J24" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K24" s="1" t="inlineStr">
-        <is>
-          <t>57600</t>
-        </is>
+      <c r="K24" s="1" t="n">
+        <v>57600</v>
       </c>
       <c r="L24" s="1">
         <f>K24/3600</f>

</xml_diff>

<commit_message>
cleared pylint and pep8 errors in sprint_report file
</commit_message>
<xml_diff>
--- a/employee-details.xlsx
+++ b/employee-details.xlsx
@@ -629,7 +629,7 @@
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J3" s="1" t="n">
@@ -648,7 +648,7 @@
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O3" s="1" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J4" s="1" t="n">
@@ -730,7 +730,7 @@
       </c>
       <c r="N4" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O4" s="1" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J5" s="1" t="n">
@@ -812,7 +812,7 @@
       </c>
       <c r="N5" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O5" s="1" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J6" s="1" t="n">
@@ -894,7 +894,7 @@
       </c>
       <c r="N6" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O6" s="1" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
       <c r="J7" s="1" t="n">
@@ -976,12 +976,12 @@
       </c>
       <c r="N7" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O7" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
       <c r="P7" s="1">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
       <c r="J8" s="1" t="n">
@@ -1058,12 +1058,12 @@
       </c>
       <c r="N8" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O8" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
       <c r="P8" s="1">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
       <c r="J9" s="1" t="n">
@@ -1140,12 +1140,12 @@
       </c>
       <c r="N9" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O9" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
       <c r="P9" s="1">
@@ -1198,12 +1198,12 @@
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="I10" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>7/13/2021</t>
         </is>
       </c>
       <c r="J10" s="1" t="n">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="N10" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="O10" s="1" t="inlineStr">
@@ -1280,12 +1280,12 @@
       </c>
       <c r="H11" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>7/13/2021</t>
         </is>
       </c>
       <c r="J11" s="1" t="n">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="N11" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="O11" s="1" t="inlineStr">
@@ -1362,12 +1362,12 @@
       </c>
       <c r="H12" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="I12" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>7/13/2021</t>
         </is>
       </c>
       <c r="J12" s="1" t="n">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="N12" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="O12" s="1" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J13" s="1" t="n">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="N13" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O13" s="1" t="inlineStr">
@@ -1526,12 +1526,12 @@
       </c>
       <c r="H14" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>7/13/2021</t>
         </is>
       </c>
       <c r="J14" s="1" t="n">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="N14" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="O14" s="1" t="inlineStr">
@@ -1608,12 +1608,12 @@
       </c>
       <c r="H15" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>7/13/2021</t>
         </is>
       </c>
       <c r="J15" s="1" t="n">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="N15" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="O15" s="1" t="inlineStr">
@@ -1695,7 +1695,7 @@
       </c>
       <c r="I16" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
       <c r="J16" s="1" t="n">
@@ -1714,12 +1714,12 @@
       </c>
       <c r="N16" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O16" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
       <c r="P16" s="1">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J17" s="1" t="n">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="N17" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O17" s="1" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="I18" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J18" s="1" t="n">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="N18" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O18" s="1" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="I19" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J19" s="1" t="n">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="N19" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O19" s="1" t="inlineStr">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="I20" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J20" s="1" t="n">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="N20" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O20" s="1" t="inlineStr">
@@ -2105,7 +2105,7 @@
       </c>
       <c r="I21" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J21" s="1" t="n">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="N21" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O21" s="1" t="inlineStr">
@@ -2182,12 +2182,12 @@
       </c>
       <c r="H22" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="I22" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>7/13/2021</t>
         </is>
       </c>
       <c r="J22" s="1" t="n">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="N22" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="O22" s="1" t="inlineStr">
@@ -2264,12 +2264,12 @@
       </c>
       <c r="H23" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="I23" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>7/13/2021</t>
         </is>
       </c>
       <c r="J23" s="1" t="n">
@@ -2288,7 +2288,7 @@
       </c>
       <c r="N23" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/4/2021</t>
         </is>
       </c>
       <c r="O23" s="1" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="I24" s="1" t="inlineStr">
         <is>
-          <t>5/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
       <c r="J24" s="1" t="n">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="N24" s="1" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>5/20/2021</t>
         </is>
       </c>
       <c r="O24" s="1" t="inlineStr">

</xml_diff>